<commit_message>
Add a script for PrimerMiner
</commit_message>
<xml_diff>
--- a/00_Data/Primers.xlsx
+++ b/00_Data/Primers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Primer</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>R.Stop</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Echinodermata</t>
   </si>
 </sst>
 </file>
@@ -423,20 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="4" max="5" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,19 +456,22 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -475,22 +484,25 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
-        <f>F2-LEN(C2)+1</f>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <f>G2-LEN(C2)+1</f>
         <v>2135</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2159</v>
       </c>
-      <c r="G2">
-        <f>H2-LEN(D2)+1</f>
+      <c r="H2">
+        <f>I2-LEN(D2)+1</f>
         <v>2818</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2839</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -503,18 +515,21 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <f>F3-LEN(C3)+1</f>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f>G3-LEN(C3)+1</f>
         <v>2329</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2348</v>
       </c>
-      <c r="G3">
-        <f>H3-LEN(D3)+1</f>
+      <c r="H3">
+        <f>I3-LEN(D3)+1</f>
         <v>3001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3020</v>
       </c>
     </row>

</xml_diff>